<commit_message>
pushing edge case validations on CRUD and pagination functionality
</commit_message>
<xml_diff>
--- a/manual_test_cases/03_Edit_or_Delete_ComputerEntry_Page_Validations.xlsx
+++ b/manual_test_cases/03_Edit_or_Delete_ComputerEntry_Page_Validations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>No</t>
   </si>
@@ -229,6 +229,9 @@
 Introduced date : 1600-02-29
 Discontinued date:2019-03-23
 Company : RCA</t>
+  </si>
+  <si>
+    <t>Home page should have records and the user clicked on a computer name link in the table</t>
   </si>
 </sst>
 </file>
@@ -296,10 +299,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,10 +633,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -658,7 +661,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -675,7 +678,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -707,7 +710,9 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
@@ -718,11 +723,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="45">
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
@@ -733,11 +740,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
@@ -748,11 +757,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
@@ -763,11 +774,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="45">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
@@ -782,7 +795,9 @@
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
@@ -793,11 +808,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="45">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>46</v>
       </c>
@@ -812,7 +829,9 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
@@ -823,11 +842,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="45">
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
@@ -842,7 +863,9 @@
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -853,11 +876,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
@@ -872,7 +897,9 @@
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>49</v>
       </c>
@@ -887,7 +914,9 @@
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
@@ -902,7 +931,9 @@
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
@@ -917,7 +948,9 @@
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>59</v>
       </c>

</xml_diff>